<commit_message>
default in wrong place
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B4FAD0-7904-AA4A-939D-4F5BA5893CA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA3F5D3-8EF3-5842-B0C5-649C90A95A5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="460" windowWidth="34400" windowHeight="28340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34400" yWindow="460" windowWidth="34400" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="client_violent_warnings" sheetId="1" r:id="rId1"/>
@@ -586,9 +586,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -864,9 +864,6 @@
       <c r="E8" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M8" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="9" spans="1:26" ht="15">
       <c r="A9" s="5" t="s">
@@ -884,6 +881,10 @@
       <c r="E9" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="M9" t="s">
+        <v>67</v>
+      </c>
+      <c r="P9" s="6"/>
     </row>
     <row r="10" spans="1:26" ht="14">
       <c r="B10" s="13"/>
@@ -2308,9 +2309,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
+      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
warnings wasn't quite right
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346F14F3-27AA-DD42-B634-67E07AB4AA87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CB8F54-355A-0948-9B04-233BF6DFDF3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="460" windowWidth="48620" windowHeight="21940" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="94">
   <si>
     <t>table_name</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>SAAR Check</t>
+  </si>
+  <si>
+    <t>OTHER</t>
   </si>
   <si>
     <t>Debt chase</t>
@@ -854,33 +857,33 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>17</v>
@@ -889,44 +892,44 @@
         <v>17</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="18" t="s">
         <v>75</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>17</v>
@@ -935,21 +938,21 @@
         <v>17</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>17</v>
@@ -958,21 +961,21 @@
         <v>17</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>17</v>
@@ -981,53 +984,53 @@
         <v>17</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>85</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1042,7 +1045,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="M5" sqref="M5:M6"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -1225,13 +1228,11 @@
       <c r="H5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="J5" s="7"/>
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -1262,13 +1263,11 @@
       <c r="H6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="J6" s="7"/>
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -1375,7 +1374,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="M5" sqref="M5:M6"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -1559,13 +1558,11 @@
         <v>40</v>
       </c>
       <c r="I5" s="7"/>
-      <c r="J5" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -1597,13 +1594,10 @@
         <v>40</v>
       </c>
       <c r="I6" s="7"/>
-      <c r="J6" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -1635,7 +1629,9 @@
         <v>40</v>
       </c>
       <c r="I7" s="7"/>
-      <c r="J7" s="4"/>
+      <c r="J7" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="K7" s="4"/>
       <c r="L7" s="8"/>
       <c r="M7" s="4"/>
@@ -2017,7 +2013,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="M5" sqref="M5:M6"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -2201,13 +2197,11 @@
         <v>29</v>
       </c>
       <c r="I5" s="7"/>
-      <c r="J5" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -2239,13 +2233,11 @@
         <v>29</v>
       </c>
       <c r="I6" s="7"/>
-      <c r="J6" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -2352,7 +2344,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5:L7"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -2536,13 +2528,11 @@
         <v>40</v>
       </c>
       <c r="I5" s="7"/>
-      <c r="J5" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -2574,13 +2564,11 @@
         <v>40</v>
       </c>
       <c r="I6" s="7"/>
-      <c r="J6" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -2688,7 +2676,7 @@
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P1" sqref="P1"/>
-      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -2872,13 +2860,11 @@
         <v>29</v>
       </c>
       <c r="I5" s="7"/>
-      <c r="J5" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -2910,13 +2896,11 @@
         <v>29</v>
       </c>
       <c r="I6" s="7"/>
-      <c r="J6" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -3024,7 +3008,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N1" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J5:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -3208,13 +3192,11 @@
         <v>29</v>
       </c>
       <c r="I5" s="7"/>
-      <c r="J5" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -3246,13 +3228,11 @@
         <v>29</v>
       </c>
       <c r="I6" s="7"/>
-      <c r="J6" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -3285,7 +3265,7 @@
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="8"/>
@@ -3432,13 +3412,13 @@
     </row>
     <row r="2" spans="1:26" ht="15">
       <c r="A2" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>19</v>
@@ -3448,18 +3428,18 @@
         <v>1</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15">
       <c r="A3" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>19</v>
@@ -3469,7 +3449,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>